<commit_message>
feat(wip): subscription list, wireframe only
</commit_message>
<xml_diff>
--- a/mockup.xlsx
+++ b/mockup.xlsx
@@ -623,8 +623,8 @@
   </sheetPr>
   <dimension ref="A3:J13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>